<commit_message>
Formatando mapa de riscos
</commit_message>
<xml_diff>
--- a/documentacao/GR01PlanoRisco.xlsx
+++ b/documentacao/GR01PlanoRisco.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Desktop\clone PI\documentacao\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas\Documents\github\projeto-pi\documentacao\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57EDCE1E-7BB1-453E-B0C2-D436FF966FCF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6BE2BB-BF69-407E-B5FB-9E0E40E6001C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{15EC4DA3-CD4A-423F-BE45-C599F9745BAB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{15EC4DA3-CD4A-423F-BE45-C599F9745BAB}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -189,7 +189,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,6 +238,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -326,7 +334,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -389,6 +397,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -729,8 +740,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EFC662F-E3D9-4E9F-B366-972CBB56BAB9}">
   <dimension ref="A1:T15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -835,7 +846,7 @@
       <c r="S3"/>
       <c r="T3"/>
     </row>
-    <row r="4" spans="1:20" s="2" customFormat="1" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" s="2" customFormat="1" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -869,7 +880,7 @@
       <c r="S4"/>
       <c r="T4"/>
     </row>
-    <row r="5" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" s="2" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -903,7 +914,7 @@
       <c r="S5"/>
       <c r="T5"/>
     </row>
-    <row r="6" spans="1:20" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" s="2" customFormat="1" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -937,7 +948,7 @@
       <c r="S6"/>
       <c r="T6"/>
     </row>
-    <row r="7" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" s="2" customFormat="1" ht="34.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -971,7 +982,7 @@
       <c r="S7"/>
       <c r="T7"/>
     </row>
-    <row r="8" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" s="2" customFormat="1" ht="37.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1005,7 +1016,7 @@
       <c r="S8"/>
       <c r="T8"/>
     </row>
-    <row r="9" spans="1:20" s="2" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" s="2" customFormat="1" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1039,7 +1050,7 @@
       <c r="S9"/>
       <c r="T9"/>
     </row>
-    <row r="10" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" s="2" customFormat="1" ht="33.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1073,7 +1084,7 @@
       <c r="S10"/>
       <c r="T10"/>
     </row>
-    <row r="11" spans="1:20" s="2" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" s="2" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="15">
         <v>10</v>
       </c>
@@ -1110,7 +1121,7 @@
     <row r="12" spans="1:20" s="2" customFormat="1" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
+      <c r="D12" s="25"/>
       <c r="E12" s="14"/>
       <c r="G12" s="18"/>
       <c r="K12"/>

</xml_diff>